<commit_message>
Added stats to the manuscript and worked on results and discussion a little bit
</commit_message>
<xml_diff>
--- a/stats_goodnessOfModel.xlsx
+++ b/stats_goodnessOfModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moin2\OneDrive\Documents\Bareground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4611122D-DB40-4E22-8A1C-49B1DFCA29A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15BEE19-F43A-4FF0-A88B-E294782C5762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7512" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{47D8B32F-EE46-4E91-B931-7F9A0F99562F}"/>
+    <workbookView xWindow="12060" yWindow="876" windowWidth="17280" windowHeight="8964" xr2:uid="{47D8B32F-EE46-4E91-B931-7F9A0F99562F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +154,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -172,10 +180,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -185,91 +194,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -610,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8607C08E-ED3F-4974-AC5E-041C61A77E4C}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +600,7 @@
       <c r="G2" s="4">
         <v>0.47699999999999998</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1122,22 +1053,53 @@
         <v>8.5000000000000006E-2</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <f>MIN(B3,B5:B8,B10:B21,B23,B25)</f>
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F27" s="2">
+        <f>MIN(F2:F25)</f>
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <f>MIN(G2:G25)</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <f>MAX(B2:B25)</f>
+        <v>0.97</v>
+      </c>
+      <c r="F28" s="2">
+        <f>MAX(F2:F25)</f>
+        <v>0.71</v>
+      </c>
+      <c r="G28" s="2">
+        <f>MAX(G2:G25)</f>
+        <v>0.94</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B25">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C25">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G25">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{AC42E49A-1E0A-44F1-9CAE-7817348B88D2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>